<commit_message>
phan quyen user and admin
</commit_message>
<xml_diff>
--- a/Bang Phan cong Cong viec.xlsx
+++ b/Bang Phan cong Cong viec.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LTDDCB_B\Baitap\doan_flutter\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="9936"/>
+    <workbookView windowWidth="22103" windowHeight="9935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>HỌC KỲ: THU 2022</t>
   </si>
@@ -140,6 +135,24 @@
   </si>
   <si>
     <t>30/5/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix code login dang nhap </t>
+  </si>
+  <si>
+    <t>4/6/2023</t>
+  </si>
+  <si>
+    <t>lam code register user va admin</t>
+  </si>
+  <si>
+    <t>5/6/2024</t>
+  </si>
+  <si>
+    <t>lam code phan quyen user va admin</t>
+  </si>
+  <si>
+    <t>6/6/2023</t>
   </si>
   <si>
     <t>Nguyễn Minh Tài</t>
@@ -166,8 +179,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,16 +221,346 @@
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -315,20 +664,298 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -336,69 +963,76 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -418,7 +1052,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -455,7 +1089,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -728,291 +1362,291 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:K30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A4:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77777777777778" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.8888888888889" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.2222222222222" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4444444444444" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" ht="20.399999999999999" customHeight="1">
-      <c r="A4" s="12" t="s">
+    <row r="4" ht="20.4" customHeight="1" spans="1:11">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.399999999999999">
-      <c r="A5" s="12" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" ht="17.4" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="21.6" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" ht="21.6" customHeight="1" spans="1:11">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="14" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="20" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="24" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" ht="52.2" customHeight="1">
-      <c r="A9" s="17" t="s">
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" ht="52.2" customHeight="1" spans="1:7">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="18" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" ht="46.8">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="6" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" ht="31.2" spans="1:8">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="7">
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="19">
         <v>2</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="7">
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="19">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="19">
         <v>2</v>
       </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="7">
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19">
         <v>3</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="19">
         <v>2</v>
       </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="7">
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="19">
         <v>4</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="19">
         <v>2</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="7">
+      <c r="A17" s="19">
         <v>5</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="19">
         <v>2</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7">
+      <c r="A18" s="19">
         <v>6</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="19">
         <v>2</v>
       </c>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -1022,10 +1656,10 @@
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="25" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="1">
@@ -1033,216 +1667,278 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="7">
+      <c r="A20" s="19">
         <v>8</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="19">
         <v>2</v>
       </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="7">
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="19">
         <v>1</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B30" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="C30" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E30" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F30" s="19">
         <v>2</v>
       </c>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="7">
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="19">
         <v>2</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="B31" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E31" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F31" s="19">
         <v>2</v>
       </c>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="7">
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="19">
         <v>3</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="B32" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E32" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F32" s="19">
         <v>2</v>
       </c>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="7">
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="19">
         <v>4</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="B33" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E33" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F33" s="19">
         <v>2</v>
       </c>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="7">
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="19">
         <v>5</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="B34" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E34" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F34" s="19">
         <v>3</v>
       </c>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="1">
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
         <v>6</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C35" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F35" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="1">
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
         <v>7</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="C36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E36" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F36" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1">
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
         <v>8</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="B37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E37" s="22">
         <v>44963</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F37" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="1">
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
         <v>9</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="25">
+      <c r="D38" s="21">
         <v>45083</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E38" s="21">
         <v>45083</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F38" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="D30" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D11:F11"/>
@@ -1251,14 +1947,10 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D8:E9"/>
     <mergeCell ref="F8:G9"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lam code register user and admin xet dieu kieu dk an hien password lam code list account user and admin , lam chuc nang crud va sua code cho dong bo du lieu bien
</commit_message>
<xml_diff>
--- a/Bang Phan cong Cong viec.xlsx
+++ b/Bang Phan cong Cong viec.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tai Cho Dien\Documents\gitcode\doan_flutter\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="9936"/>
+    <workbookView windowWidth="22103" windowHeight="9935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
   <si>
     <t>HỌC KỲ: THU 2022</t>
   </si>
@@ -158,6 +153,18 @@
   </si>
   <si>
     <t>6/6/2023</t>
+  </si>
+  <si>
+    <t>lam code register user va admin ẩn hiện password</t>
+  </si>
+  <si>
+    <t>8/6/2023</t>
+  </si>
+  <si>
+    <t>lam code register user va admin xét điều kiện đăng ký</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lam code list account user &amp; admin ,crud cho đồng bộ dữ liệu </t>
   </si>
   <si>
     <t>Nguyễn Minh Tài</t>
@@ -187,8 +194,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,16 +236,346 @@
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -336,20 +679,298 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -357,70 +978,76 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -440,7 +1067,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -477,7 +1104,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -485,7 +1112,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6540500" y="154305"/>
+          <a:off x="7393940" y="154305"/>
           <a:ext cx="1076960" cy="396240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -750,291 +1377,291 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A4:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77777777777778" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5555555555556" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.8888888888889" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.2222222222222" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4444444444444" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" ht="20.399999999999999" customHeight="1">
-      <c r="A4" s="14" t="s">
+    <row r="4" ht="20.4" customHeight="1" spans="1:11">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.399999999999999">
-      <c r="A5" s="14" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" ht="17.4" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="21.6" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" ht="21.6" customHeight="1" spans="1:11">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="16" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="22" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="26" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" ht="52.2" customHeight="1">
-      <c r="A9" s="19" t="s">
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" ht="52.2" customHeight="1" spans="1:7">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="20" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" ht="46.8">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="6" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" ht="31.2" spans="1:8">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="7">
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="19">
         <v>2</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="7">
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="19">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="19">
         <v>2</v>
       </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="7">
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19">
         <v>3</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="19">
         <v>2</v>
       </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="7">
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="19">
         <v>4</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="19">
         <v>2</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="7">
+      <c r="A17" s="19">
         <v>5</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="19">
         <v>2</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7">
+      <c r="A18" s="19">
         <v>6</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="19">
         <v>2</v>
       </c>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -1044,10 +1671,10 @@
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="25" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="1">
@@ -1055,27 +1682,27 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="7">
+      <c r="A20" s="19">
         <v>8</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="19">
         <v>2</v>
       </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -1085,17 +1712,17 @@
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="25" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1105,17 +1732,17 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="26" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -1125,130 +1752,190 @@
       <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="25" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="1">
         <v>8</v>
       </c>
     </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+    </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="7">
+      <c r="A30" s="19">
         <v>1</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="C30" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="19">
         <v>2</v>
       </c>
-      <c r="G30" s="7"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="7">
+      <c r="A31" s="19">
         <v>2</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="10" t="s">
+      <c r="B31" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="19">
         <v>2</v>
       </c>
-      <c r="G31" s="7"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="7">
+      <c r="A32" s="19">
         <v>3</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="B32" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="19">
         <v>2</v>
       </c>
-      <c r="G32" s="7"/>
+      <c r="G32" s="19"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="7">
+      <c r="A33" s="19">
         <v>4</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="B33" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="19">
         <v>2</v>
       </c>
-      <c r="G33" s="7"/>
+      <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="7">
+      <c r="A34" s="19">
         <v>5</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="19">
         <v>3</v>
       </c>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>46</v>
+      <c r="C35" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>34</v>
@@ -1256,11 +1943,11 @@
       <c r="E35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>7</v>
       </c>
@@ -1268,72 +1955,72 @@
         <v>36</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="25" t="s">
         <v>37</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="22">
         <v>44963</v>
       </c>
       <c r="F37" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="8">
+        <v>50</v>
+      </c>
+      <c r="D38" s="21">
         <v>45083</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="21">
         <v>45083</v>
       </c>
       <c r="F38" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="8">
+        <v>50</v>
+      </c>
+      <c r="D39" s="21">
         <v>45113</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="21">
         <v>45113</v>
       </c>
       <c r="F39" s="1">
@@ -1342,6 +2029,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D11:F11"/>
@@ -1350,14 +2042,10 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D8:E9"/>
     <mergeCell ref="F8:G9"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
gan lap trinh user admin crud register vo giao dien
</commit_message>
<xml_diff>
--- a/Bang Phan cong Cong viec.xlsx
+++ b/Bang Phan cong Cong viec.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>HỌC KỲ: THU 2022</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t xml:space="preserve">lam code list account user &amp; admin ,crud cho đồng bộ dữ liệu </t>
+  </si>
+  <si>
+    <t>gan lap trinh user admin crud register vo giao dien</t>
+  </si>
+  <si>
+    <t>9/6/2023</t>
   </si>
   <si>
     <t>Nguyễn Minh Tài</t>
@@ -196,10 +202,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -238,16 +244,55 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -259,14 +304,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -290,14 +327,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -307,16 +336,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,7 +352,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -345,7 +366,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,28 +386,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -390,187 +396,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,17 +686,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,17 +725,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -766,29 +783,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -798,130 +804,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1383,10 +1389,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A4:K39"/>
+  <dimension ref="A4:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.6"/>
@@ -1822,208 +1828,238 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="19">
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="7:7">
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="7:7">
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="7:7">
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="7:7">
+      <c r="G34" s="19"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="19">
         <v>1</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B38" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="23" t="s">
+      <c r="C38" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E38" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F38" s="19">
         <v>2</v>
       </c>
-      <c r="G30" s="19"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="19">
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="19">
         <v>2</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="23" t="s">
+      <c r="B39" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E39" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F39" s="19">
         <v>2</v>
       </c>
-      <c r="G31" s="19"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="19">
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="19">
         <v>3</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B40" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="23" t="s">
+      <c r="D40" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E40" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F40" s="19">
         <v>2</v>
       </c>
-      <c r="G32" s="19"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="19">
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="19">
         <v>4</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="23" t="s">
+      <c r="B41" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E41" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F41" s="19">
         <v>2</v>
       </c>
-      <c r="G33" s="19"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="19">
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="19">
         <v>5</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="23" t="s">
+      <c r="B42" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E42" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F42" s="19">
         <v>3</v>
       </c>
-      <c r="G34" s="19"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1">
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1">
         <v>6</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="C43" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F43" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="1">
+    <row r="44" spans="1:6">
+      <c r="A44" s="1">
         <v>7</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="25" t="s">
+      <c r="C44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E44" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F44" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1">
+    <row r="45" spans="1:6">
+      <c r="A45" s="1">
         <v>8</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="19" t="s">
+      <c r="B45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="22">
+      <c r="E45" s="22">
         <v>44963</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F45" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="1">
+    <row r="46" spans="1:6">
+      <c r="A46" s="1">
         <v>9</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="21">
+      <c r="B46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="21">
         <v>45083</v>
       </c>
-      <c r="E38" s="21">
+      <c r="E46" s="21">
         <v>45083</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F46" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="1">
+    <row r="47" spans="1:6">
+      <c r="A47" s="1">
         <v>10</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="21">
+      <c r="B47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="21">
         <v>45113</v>
       </c>
-      <c r="E39" s="21">
+      <c r="E47" s="21">
         <v>45113</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F47" s="1">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lam giao dien profile , theme dark ,light code chuc nang profile , theme dark ,light
</commit_message>
<xml_diff>
--- a/Bang Phan cong Cong viec.xlsx
+++ b/Bang Phan cong Cong viec.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LTDDCB_B\Baitap\New folder\Nhom3_ShopOnl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="9936"/>
+    <workbookView windowWidth="22103" windowHeight="9935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>HỌC KỲ: THU 2022</t>
   </si>
@@ -178,6 +173,12 @@
     <t>9/6/2023</t>
   </si>
   <si>
+    <t xml:space="preserve">lam giao dien profile , theme dark light va code chuc nang </t>
+  </si>
+  <si>
+    <t>10/6/2023</t>
+  </si>
+  <si>
     <t>Nguyễn Minh Tài</t>
   </si>
   <si>
@@ -191,9 +192,6 @@
   </si>
   <si>
     <t>category hiện thị và xem thông tin sản phẩm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> login làm code backend</t>
   </si>
   <si>
     <t>lấy dữ liệu và hiển thị thông tin, thêm tạo thông tin</t>
@@ -208,8 +206,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,16 +248,346 @@
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -357,20 +691,298 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,70 +990,75 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -461,7 +1078,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -498,7 +1115,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -771,291 +1388,291 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:K48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A4:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77777777777778" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5555555555556" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.8888888888889" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.2222222222222" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4444444444444" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" ht="20.399999999999999" customHeight="1">
-      <c r="A4" s="14" t="s">
+    <row r="4" ht="20.4" customHeight="1" spans="1:11">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.399999999999999">
-      <c r="A5" s="14" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" ht="17.4" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="21.6" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" ht="21.6" customHeight="1" spans="1:11">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="16" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="22" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="26" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" ht="52.2" customHeight="1">
-      <c r="A9" s="19" t="s">
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" ht="52.2" customHeight="1" spans="1:7">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="20" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" ht="46.8">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="6" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" ht="31.2" spans="1:8">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="7">
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="19">
         <v>2</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="7">
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="19">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="19">
         <v>2</v>
       </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="7">
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19">
         <v>3</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="19">
         <v>2</v>
       </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="7">
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="19">
         <v>4</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="19">
         <v>2</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="7">
+      <c r="A17" s="19">
         <v>5</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="19">
         <v>2</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7">
+      <c r="A18" s="19">
         <v>6</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="19">
         <v>2</v>
       </c>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -1065,10 +1682,10 @@
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="24" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="1">
@@ -1076,27 +1693,27 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="7">
+      <c r="A20" s="19">
         <v>8</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="19">
         <v>2</v>
       </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -1106,17 +1723,17 @@
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="24" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1126,17 +1743,17 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -1146,17 +1763,17 @@
       <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="24" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -1166,17 +1783,17 @@
       <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -1186,17 +1803,17 @@
       <c r="C25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>14</v>
       </c>
@@ -1206,17 +1823,17 @@
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F26" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>15</v>
       </c>
@@ -1226,140 +1843,160 @@
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="24" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="G34" s="7"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="7">
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="7:7">
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="7:7">
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="7:7">
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="7:7">
+      <c r="G34" s="19"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="19">
         <v>1</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="C38" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="7">
+    <row r="39" spans="1:6">
+      <c r="A39" s="19">
         <v>2</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="10" t="s">
+      <c r="B39" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="7">
+    <row r="40" spans="1:6">
+      <c r="A40" s="19">
         <v>3</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="7">
+    <row r="41" spans="1:6">
+      <c r="A41" s="19">
         <v>4</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="10" t="s">
+      <c r="B41" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="7">
+    <row r="42" spans="1:6">
+      <c r="A42" s="19">
         <v>5</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>56</v>
+      <c r="B42" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>52</v>
+      <c r="C43" s="19" t="s">
+        <v>54</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>34</v>
@@ -1367,11 +2004,11 @@
       <c r="E43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>7</v>
       </c>
@@ -1379,100 +2016,85 @@
         <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="24" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="9">
-        <v>44963</v>
+        <v>54</v>
+      </c>
+      <c r="D45" s="21">
+        <v>45083</v>
+      </c>
+      <c r="E45" s="21">
+        <v>45083</v>
       </c>
       <c r="F45" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>9</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="8">
-        <v>45083</v>
-      </c>
-      <c r="E46" s="8">
-        <v>45083</v>
+        <v>54</v>
+      </c>
+      <c r="D46" s="21">
+        <v>45113</v>
+      </c>
+      <c r="E46" s="21">
+        <v>45113</v>
       </c>
       <c r="F46" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="8">
-        <v>45113</v>
-      </c>
-      <c r="E47" s="8">
-        <v>45113</v>
+        <v>54</v>
+      </c>
+      <c r="D47" s="21">
+        <v>45205</v>
+      </c>
+      <c r="E47" s="21">
+        <v>45205</v>
       </c>
       <c r="F47" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="1">
-        <v>11</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="8">
-        <v>45205</v>
-      </c>
-      <c r="E48" s="8">
-        <v>45205</v>
-      </c>
-      <c r="F48" s="1">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D11:F11"/>
@@ -1481,14 +2103,10 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D8:E9"/>
     <mergeCell ref="F8:G9"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lam profile chua xong
</commit_message>
<xml_diff>
--- a/Bang Phan cong Cong viec.xlsx
+++ b/Bang Phan cong Cong viec.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
   <si>
     <t>HỌC KỲ: THU 2022</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>10/6/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chua xong </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lam profile </t>
+  </si>
+  <si>
+    <t>12/6/2023</t>
   </si>
   <si>
     <t>Nguyễn Minh Tài</t>
@@ -208,10 +217,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -250,14 +259,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,6 +289,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -281,25 +322,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -327,54 +352,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -387,11 +368,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -402,187 +411,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,6 +702,45 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -726,55 +774,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -789,10 +789,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -810,130 +819,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1396,8 +1405,8 @@
   <sheetPr/>
   <dimension ref="A4:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.6"/>
@@ -1853,7 +1862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>16</v>
       </c>
@@ -1871,6 +1880,32 @@
       </c>
       <c r="F28" s="1">
         <v>4</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1">
+        <v>17</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="1">
+        <v>6</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="7:7">
@@ -1896,7 +1931,7 @@
         <v>18</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>20</v>
@@ -1913,10 +1948,10 @@
         <v>2</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>22</v>
@@ -1933,10 +1968,10 @@
         <v>3</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>25</v>
@@ -1953,10 +1988,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>54</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>28</v>
@@ -1973,10 +2008,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>31</v>
@@ -1996,7 +2031,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>34</v>
@@ -2016,7 +2051,7 @@
         <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D44" s="24" t="s">
         <v>37</v>
@@ -2033,10 +2068,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D45" s="21">
         <v>45083</v>
@@ -2053,10 +2088,10 @@
         <v>9</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D46" s="21">
         <v>45113</v>
@@ -2073,10 +2108,10 @@
         <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D47" s="21">
         <v>45205</v>

</xml_diff>

<commit_message>
sua lai giao dien va phan trang nguoi dung , chinh lai menu khi nguoi dung dang nhap vao co ten nguoi dung
</commit_message>
<xml_diff>
--- a/Bang Phan cong Cong viec.xlsx
+++ b/Bang Phan cong Cong viec.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>HỌC KỲ: THU 2022</t>
   </si>
@@ -173,7 +173,7 @@
     <t>9/6/2023</t>
   </si>
   <si>
-    <t xml:space="preserve">lam giao dien profile , theme dark light va code chuc nang </t>
+    <t>lam giao dien profile , theme dark light</t>
   </si>
   <si>
     <t>10/6/2023</t>
@@ -182,12 +182,24 @@
     <t xml:space="preserve">chua xong </t>
   </si>
   <si>
-    <t xml:space="preserve">lam profile </t>
+    <t xml:space="preserve">lam profile va code chuc nang </t>
   </si>
   <si>
     <t>12/6/2023</t>
   </si>
   <si>
+    <t>Làm code search để tìm kiếm sản phẩm</t>
+  </si>
+  <si>
+    <t>13/6/2023</t>
+  </si>
+  <si>
+    <t>lam login phan trang va sua lai menu luc dang nhap co ten nguoi dung</t>
+  </si>
+  <si>
+    <t>15/6/2023</t>
+  </si>
+  <si>
     <t>Nguyễn Minh Tài</t>
   </si>
   <si>
@@ -210,6 +222,9 @@
   </si>
   <si>
     <t>Lấy dữ liệu hình và thông tin và hiển thị products</t>
+  </si>
+  <si>
+    <t>Thêm tăng giảm số lượng sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -217,9 +232,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -260,6 +275,98 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,6 +380,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -281,126 +410,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -411,187 +426,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,6 +716,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -725,17 +755,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,26 +779,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -789,19 +813,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -822,127 +837,127 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1132,7 +1147,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7393940" y="154305"/>
+          <a:off x="7843520" y="154305"/>
           <a:ext cx="1076960" cy="396240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1403,16 +1418,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A4:K47"/>
+  <dimension ref="A4:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="4.77777777777778" style="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5555555555556" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.1111111111111" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.8888888888889" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.2222222222222" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.4444444444444" style="1" customWidth="1"/>
@@ -1908,10 +1923,46 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="7:7">
+    <row r="30" spans="1:7">
+      <c r="A30" s="1">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3</v>
+      </c>
       <c r="G30" s="19"/>
     </row>
-    <row r="31" spans="7:7">
+    <row r="31" spans="1:7">
+      <c r="A31" s="1">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="1">
+        <v>4</v>
+      </c>
       <c r="G31" s="19"/>
     </row>
     <row r="32" spans="7:7">
@@ -1931,7 +1982,7 @@
         <v>18</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>20</v>
@@ -1948,10 +1999,10 @@
         <v>2</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>22</v>
@@ -1968,10 +2019,10 @@
         <v>3</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>25</v>
@@ -1988,10 +2039,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>28</v>
@@ -2008,10 +2059,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>31</v>
@@ -2031,7 +2082,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>34</v>
@@ -2051,7 +2102,7 @@
         <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D44" s="24" t="s">
         <v>37</v>
@@ -2068,10 +2119,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D45" s="21">
         <v>45083</v>
@@ -2088,10 +2139,10 @@
         <v>9</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D46" s="21">
         <v>45113</v>
@@ -2108,10 +2159,10 @@
         <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D47" s="21">
         <v>45205</v>
@@ -2121,6 +2172,46 @@
       </c>
       <c r="F47" s="1">
         <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1">
+        <v>11</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="21">
+        <v>45266</v>
+      </c>
+      <c r="E48" s="21">
+        <v>45266</v>
+      </c>
+      <c r="F48" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Làm thêm sản phẩm, xóa sản phẩm và tăng giảm số lượng trong giỏ hàng
</commit_message>
<xml_diff>
--- a/Bang Phan cong Cong viec.xlsx
+++ b/Bang Phan cong Cong viec.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tai Cho Dien\Documents\gitcode\Nhom3_ShopOnl\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="22103" windowHeight="9935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="9936"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="71">
   <si>
     <t>HỌC KỲ: THU 2022</t>
   </si>
@@ -225,19 +230,16 @@
   </si>
   <si>
     <t>Thêm tăng giảm số lượng sản phẩm</t>
+  </si>
+  <si>
+    <t>Làm thêm sản phẩm, xóa sản phẩm, tăng giảm sản phẩm trong giỏ hàng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,346 +274,16 @@
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -715,259 +387,35 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -980,20 +428,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1001,88 +449,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1102,7 +490,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1139,7 +527,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1412,291 +800,291 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A4:K49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="4.77777777777778" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64.1111111111111" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.8888888888889" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.2222222222222" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.4444444444444" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88888888888889" style="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" ht="20.4" customHeight="1" spans="1:11">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:11" ht="20.399999999999999" customHeight="1">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" ht="17.4" spans="1:11">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.399999999999999">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" ht="21.6" customHeight="1" spans="1:11">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="21.6" customHeight="1">
+      <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="5" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" ht="52.2" customHeight="1" spans="1:7">
-      <c r="A9" s="11" t="s">
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:11" ht="52.2" customHeight="1">
+      <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="15" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" ht="31.2" spans="1:8">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="18" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="46.8">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="19">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="7">
         <v>1</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="22" t="s">
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="7">
         <v>2</v>
       </c>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="19">
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="22" t="s">
+      <c r="C14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="7">
         <v>2</v>
       </c>
-      <c r="G14" s="19"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="19">
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="7">
         <v>3</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="7">
         <v>2</v>
       </c>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="19">
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="7">
         <v>4</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="22" t="s">
+      <c r="C16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="7">
         <v>2</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="19">
+      <c r="A17" s="7">
         <v>5</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="C17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="7">
         <v>2</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="19">
+      <c r="A18" s="7">
         <v>6</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="22" t="s">
+      <c r="C18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="7">
         <v>2</v>
       </c>
-      <c r="G18" s="19"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -1706,10 +1094,10 @@
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="1">
@@ -1717,27 +1105,27 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="19">
+      <c r="A20" s="7">
         <v>8</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="7">
         <v>2</v>
       </c>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -1747,17 +1135,17 @@
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="11" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1767,17 +1155,17 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="12" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -1787,17 +1175,17 @@
       <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="11" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -1807,17 +1195,17 @@
       <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="11" t="s">
         <v>47</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -1827,17 +1215,17 @@
       <c r="C25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="11" t="s">
         <v>47</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>14</v>
       </c>
@@ -1847,17 +1235,17 @@
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="11" t="s">
         <v>47</v>
       </c>
       <c r="F26" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>15</v>
       </c>
@@ -1867,10 +1255,10 @@
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="1">
@@ -1887,10 +1275,10 @@
       <c r="C28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="11" t="s">
         <v>53</v>
       </c>
       <c r="F28" s="1">
@@ -1910,10 +1298,10 @@
       <c r="C29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="11" t="s">
         <v>56</v>
       </c>
       <c r="F29" s="1">
@@ -1942,7 +1330,7 @@
       <c r="F30" s="1">
         <v>3</v>
       </c>
-      <c r="G30" s="19"/>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1">
@@ -1954,134 +1342,151 @@
       <c r="C31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="11" t="s">
         <v>60</v>
       </c>
       <c r="F31" s="1">
         <v>4</v>
       </c>
-      <c r="G31" s="19"/>
-    </row>
-    <row r="32" spans="7:7">
-      <c r="G32" s="19"/>
-    </row>
-    <row r="33" spans="7:7">
-      <c r="G33" s="19"/>
-    </row>
-    <row r="34" spans="7:7">
-      <c r="G34" s="19"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="19">
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="G34" s="7"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="7">
         <v>1</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="19">
+      <c r="F38" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="19">
+    <row r="39" spans="1:7">
+      <c r="A39" s="7">
         <v>2</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F39" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="19">
+    <row r="40" spans="1:7">
+      <c r="A40" s="7">
         <v>3</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="19">
+      <c r="F40" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="19">
+    <row r="41" spans="1:7">
+      <c r="A41" s="7">
         <v>4</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="23" t="s">
+      <c r="E41" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="19">
+    <row r="42" spans="1:7">
+      <c r="A42" s="7">
         <v>5</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="23" t="s">
+      <c r="E42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F42" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="7" t="s">
         <v>61</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2090,11 +1495,11 @@
       <c r="E43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F43" s="19">
+      <c r="F43" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>7</v>
       </c>
@@ -2104,17 +1509,17 @@
       <c r="C44" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D44" s="24" t="s">
+      <c r="D44" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E44" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>8</v>
       </c>
@@ -2124,17 +1529,17 @@
       <c r="C45" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="21">
+      <c r="D45" s="8">
         <v>45083</v>
       </c>
-      <c r="E45" s="21">
+      <c r="E45" s="8">
         <v>45083</v>
       </c>
       <c r="F45" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
         <v>9</v>
       </c>
@@ -2144,17 +1549,17 @@
       <c r="C46" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D46" s="21">
+      <c r="D46" s="8">
         <v>45113</v>
       </c>
-      <c r="E46" s="21">
+      <c r="E46" s="8">
         <v>45113</v>
       </c>
       <c r="F46" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
         <v>10</v>
       </c>
@@ -2164,17 +1569,17 @@
       <c r="C47" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="8">
         <v>45205</v>
       </c>
-      <c r="E47" s="21">
+      <c r="E47" s="8">
         <v>45205</v>
       </c>
       <c r="F47" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
         <v>11</v>
       </c>
@@ -2184,10 +1589,10 @@
       <c r="C48" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="8">
         <v>45266</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E48" s="8">
         <v>45266</v>
       </c>
       <c r="F48" s="1">
@@ -2214,13 +1619,28 @@
         <v>3</v>
       </c>
     </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1">
+        <v>13</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" s="1">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D11:F11"/>
@@ -2229,10 +1649,14 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D8:E9"/>
     <mergeCell ref="F8:G9"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
làm tínnh tổng tiền của giỏ hàng
</commit_message>
<xml_diff>
--- a/Bang Phan cong Cong viec.xlsx
+++ b/Bang Phan cong Cong viec.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tai Cho Dien\Documents\gitcode\Nhom3_ShopOnl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="9936"/>
+    <workbookView windowWidth="22103" windowHeight="9935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
   <si>
     <t>HỌC KỲ: THU 2022</t>
   </si>
@@ -205,6 +200,12 @@
     <t>15/6/2023</t>
   </si>
   <si>
+    <t>Làm thêm sản phẩm, xóa sản phẩm, tăng giảm sản phẩm trong giỏ hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">làm tính tổng tiền của giỏ hàng </t>
+  </si>
+  <si>
     <t>Nguyễn Minh Tài</t>
   </si>
   <si>
@@ -230,16 +231,19 @@
   </si>
   <si>
     <t>Thêm tăng giảm số lượng sản phẩm</t>
-  </si>
-  <si>
-    <t>Làm thêm sản phẩm, xóa sản phẩm, tăng giảm sản phẩm trong giỏ hàng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,16 +278,346 @@
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -387,20 +721,298 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -408,69 +1020,75 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -490,7 +1108,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -527,7 +1145,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -800,291 +1418,291 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:K50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A4:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77777777777778" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.8888888888889" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.2222222222222" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4444444444444" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" ht="20.399999999999999" customHeight="1">
-      <c r="A4" s="13" t="s">
+    <row r="4" ht="20.4" customHeight="1" spans="1:11">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.399999999999999">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" ht="17.4" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="21.6" customHeight="1">
-      <c r="A7" s="14" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" ht="21.6" customHeight="1" spans="1:11">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="15" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="21" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="25" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="22"/>
-    </row>
-    <row r="9" spans="1:11" ht="52.2" customHeight="1">
-      <c r="A9" s="18" t="s">
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" ht="52.2" customHeight="1" spans="1:7">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="19" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" ht="46.8">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="6" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" ht="31.2" spans="1:8">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="7">
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="19">
         <v>2</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="7">
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="19">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="19">
         <v>2</v>
       </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="7">
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19">
         <v>3</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="19">
         <v>2</v>
       </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="7">
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="19">
         <v>4</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="19">
         <v>2</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="7">
+      <c r="A17" s="19">
         <v>5</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="19">
         <v>2</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7">
+      <c r="A18" s="19">
         <v>6</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="19">
         <v>2</v>
       </c>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -1094,10 +1712,10 @@
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="24" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="1">
@@ -1105,27 +1723,27 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="7">
+      <c r="A20" s="19">
         <v>8</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="19">
         <v>2</v>
       </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -1135,17 +1753,17 @@
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="24" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1155,17 +1773,17 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -1175,17 +1793,17 @@
       <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="24" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -1195,17 +1813,17 @@
       <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -1215,17 +1833,17 @@
       <c r="C25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>14</v>
       </c>
@@ -1235,17 +1853,17 @@
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F26" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>15</v>
       </c>
@@ -1255,10 +1873,10 @@
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="24" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="1">
@@ -1275,10 +1893,10 @@
       <c r="C28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="24" t="s">
         <v>53</v>
       </c>
       <c r="F28" s="1">
@@ -1298,10 +1916,10 @@
       <c r="C29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="24" t="s">
         <v>56</v>
       </c>
       <c r="F29" s="1">
@@ -1330,7 +1948,7 @@
       <c r="F30" s="1">
         <v>3</v>
       </c>
-      <c r="G30" s="7"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1">
@@ -1342,23 +1960,23 @@
       <c r="C31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="24" t="s">
         <v>60</v>
       </c>
       <c r="F31" s="1">
         <v>4</v>
       </c>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>20</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>19</v>
@@ -1374,120 +1992,138 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="G34" s="7"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="7">
+      <c r="A33" s="1">
+        <v>21</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="1">
         <v>1</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="7:7">
+      <c r="G34" s="19"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="19">
+        <v>1</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D38" s="9" t="s">
+      <c r="C38" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="7">
+    <row r="39" spans="1:6">
+      <c r="A39" s="19">
         <v>2</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D39" s="9" t="s">
+      <c r="B39" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="7">
+    <row r="40" spans="1:6">
+      <c r="A40" s="19">
         <v>3</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="7">
+    <row r="41" spans="1:6">
+      <c r="A41" s="19">
         <v>4</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="9" t="s">
+      <c r="B41" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="7">
+    <row r="42" spans="1:6">
+      <c r="A42" s="19">
         <v>5</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>65</v>
+      <c r="B42" s="19" t="s">
+        <v>67</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D42" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>61</v>
+      <c r="C43" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>34</v>
@@ -1495,11 +2131,11 @@
       <c r="E43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>7</v>
       </c>
@@ -1507,92 +2143,92 @@
         <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="24" t="s">
         <v>37</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" s="8">
+        <v>63</v>
+      </c>
+      <c r="D45" s="21">
         <v>45083</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="21">
         <v>45083</v>
       </c>
       <c r="F45" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>9</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="8">
+        <v>63</v>
+      </c>
+      <c r="D46" s="21">
         <v>45113</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="21">
         <v>45113</v>
       </c>
       <c r="F46" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="8">
+        <v>63</v>
+      </c>
+      <c r="D47" s="21">
         <v>45205</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47" s="21">
         <v>45205</v>
       </c>
       <c r="F47" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>11</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" s="8">
+        <v>63</v>
+      </c>
+      <c r="D48" s="21">
         <v>45266</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="21">
         <v>45266</v>
       </c>
       <c r="F48" s="1">
@@ -1607,7 +2243,7 @@
         <v>57</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>58</v>
@@ -1624,10 +2260,10 @@
         <v>13</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>60</v>
@@ -1639,8 +2275,33 @@
         <v>5</v>
       </c>
     </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1">
+        <v>14</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D11:F11"/>
@@ -1649,14 +2310,10 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D8:E9"/>
     <mergeCell ref="F8:G9"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>